<commit_message>
Php feladat elkezdve home nézet megoldva
</commit_message>
<xml_diff>
--- a/beugro.xlsx
+++ b/beugro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momsz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momsz/Desktop/Git/Beugro_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101D5611-F858-CF44-A481-70F1737B20D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F421000-AFFB-8C47-9423-A13F7D84373A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="1" xr2:uid="{569F5DE4-A08A-4C8B-B149-0E3A1A40B1BA}"/>
+    <workbookView xWindow="-25600" yWindow="3380" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{569F5DE4-A08A-4C8B-B149-0E3A1A40B1BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feladat1" sheetId="1" r:id="rId1"/>
@@ -462,23 +462,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -681,9 +681,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>363220</xdr:colOff>
+          <xdr:colOff>368300</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>103777</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1094,33 +1094,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -1129,12 +1129,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="E4" s="8" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="E4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
@@ -1142,22 +1142,22 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="E5" s="8"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="E5" s="9"/>
       <c r="F5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="E6" t="s">
         <v>10</v>
       </c>
@@ -1166,11 +1166,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1179,11 +1179,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1200,11 +1200,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1213,11 +1213,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1235,7 +1235,7 @@
       <c r="C12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1253,7 +1253,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>57</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="C15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="C16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="C17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>63</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1357,8 +1357,8 @@
         <v>64</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F19" t="s">
@@ -1366,18 +1366,18 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="9"/>
       <c r="F20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="C22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F22" t="s">
@@ -1410,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="9"/>
       <c r="F23" t="s">
         <v>45</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F24" t="s">
@@ -1433,18 +1433,18 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="E25" s="8"/>
+      <c r="E25" s="9"/>
       <c r="F25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="E26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="9"/>
       <c r="F26" t="s">
         <v>47</v>
       </c>
@@ -1526,6 +1526,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E22:E23"/>
@@ -1542,9 +1545,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="D12:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="E19:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043BB768-4C59-4B55-9AAF-2B6CB27158DD}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1569,26 +1569,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
@@ -1625,11 +1625,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1864,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBC8EF8-F127-4B2C-A403-72C3E2B4CA9E}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1877,26 +1877,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
@@ -1920,11 +1920,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>